<commit_message>
hehe checking this out
</commit_message>
<xml_diff>
--- a/INVENTARIO.xlsx
+++ b/INVENTARIO.xlsx
@@ -11,27 +11,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Coca</t>
   </si>
   <si>
-    <t>15</t>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Pan</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>40</t>
   </si>
   <si>
     <t>60</t>
   </si>
   <si>
-    <t>Agua</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -39,12 +48,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -66,10 +76,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -366,7 +377,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -375,47 +386,69 @@
   <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="B3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made more changes, i need to figure out how to know when to use "nuevo()" or "usado()"
</commit_message>
<xml_diff>
--- a/INVENTARIO.xlsx
+++ b/INVENTARIO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Coca</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>Fanta</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +457,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
agregue venderItem(), en la linea 68, agregue y termine IVesta(), funcion que decide si el item que se vendio ya se habia vendido o no, agregue y termine IVusado(), funcion que se ejecuta si el item vendido ya se habia vendido con anterioridad. No probe ninguna
</commit_message>
<xml_diff>
--- a/INVENTARIO.xlsx
+++ b/INVENTARIO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Coca</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>Tang</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -390,7 +396,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="n">
         <v>40</v>
@@ -449,6 +455,17 @@
       </c>
       <c r="C6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully finished venderItem(), next one is editarFile(), viva el vino
</commit_message>
<xml_diff>
--- a/INVENTARIO.xlsx
+++ b/INVENTARIO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Coca</t>
   </si>
@@ -19,6 +19,9 @@
     <t>Agua</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>Pan</t>
   </si>
   <si>
@@ -34,10 +37,13 @@
     <t>Fanta</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Vino</t>
   </si>
   <si>
-    <t>30</t>
+    <t>25</t>
   </si>
   <si>
     <t>27</t>
@@ -47,6 +53,12 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>Pitusas</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,8 +418,8 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>20</v>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>50</v>
@@ -415,7 +427,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20</v>
@@ -426,46 +438,57 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes on the excel files
</commit_message>
<xml_diff>
--- a/INVENTARIO.xlsx
+++ b/INVENTARIO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Coca</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>Blem</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -407,7 +410,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="1" t="n">
@@ -489,6 +492,17 @@
       </c>
       <c r="C8" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a feature: when a item is selled, it shows how many item are left in inventory
</commit_message>
<xml_diff>
--- a/INVENTARIO.xlsx
+++ b/INVENTARIO.xlsx
@@ -16,6 +16,9 @@
     <t>Coca</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Agua</t>
   </si>
   <si>
@@ -35,9 +38,6 @@
   </si>
   <si>
     <t>Fanta</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>Vino</t>
@@ -411,7 +411,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="n">
         <v>40</v>
@@ -419,10 +419,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>50</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20</v>
@@ -441,24 +441,24 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -477,7 +477,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -488,7 +488,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -499,10 +499,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>